<commit_message>
recalculated LSTMs without aux input
</commit_message>
<xml_diff>
--- a/Results/Accuracies.xlsx
+++ b/Results/Accuracies.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\BISS\MSc Thesis\Data\Anonymized Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\BISS\MSc Thesis\GitHub\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracies + Sens 3 Classes" sheetId="2" r:id="rId1"/>
@@ -1206,7 +1206,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1232,7 +1231,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1738,7 +1737,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -1829,7 +1828,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1861,7 +1860,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -1878,7 +1877,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1904,7 +1902,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1934,7 +1932,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1989,7 +1987,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2015,7 +2012,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2454,7 +2451,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -2546,7 +2543,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2578,7 +2575,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -2595,7 +2592,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2621,7 +2617,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2651,7 +2647,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2731,7 +2727,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3170,7 +3166,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -3262,7 +3258,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3294,7 +3290,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -3336,7 +3332,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3366,7 +3362,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3446,7 +3442,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3885,7 +3881,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -3977,7 +3973,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4009,7 +4005,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -4051,7 +4047,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4081,7 +4077,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4136,7 +4132,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4162,7 +4157,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4668,7 +4663,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -4759,7 +4754,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4791,7 +4786,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -4808,7 +4803,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4834,7 +4828,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4864,7 +4858,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4919,7 +4913,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4945,7 +4938,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5451,7 +5444,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -5542,7 +5535,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5574,7 +5567,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -5591,7 +5584,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5617,7 +5609,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5647,7 +5639,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5702,7 +5694,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5728,7 +5719,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6167,7 +6158,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -6259,7 +6250,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6291,7 +6282,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -6308,7 +6299,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6334,7 +6324,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6364,7 +6354,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6419,7 +6409,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6445,7 +6434,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6884,7 +6873,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -6976,7 +6965,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7008,7 +6997,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -7025,7 +7014,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7051,7 +7039,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7081,7 +7069,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7136,7 +7124,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7162,7 +7149,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7601,7 +7588,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -7693,7 +7680,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7725,7 +7712,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -7742,7 +7729,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7768,7 +7754,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7798,7 +7784,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7878,7 +7864,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8384,7 +8370,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -8475,7 +8461,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8507,7 +8493,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -8549,7 +8535,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8579,7 +8565,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8634,7 +8620,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8660,7 +8645,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9166,7 +9151,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -9257,7 +9242,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9289,7 +9274,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -9306,7 +9291,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9332,7 +9316,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9362,7 +9346,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9442,7 +9426,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9948,7 +9932,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463246576"/>
@@ -10039,7 +10023,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10071,7 +10055,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1463251152"/>
@@ -10113,7 +10097,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -10143,7 +10127,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16843,7 +16827,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -16873,7 +16863,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -16905,7 +16901,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -16937,7 +16939,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -16969,7 +16977,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -17001,7 +17015,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -17038,7 +17058,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -17070,7 +17096,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvPr id="15" name="Chart 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -17102,7 +17134,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="16" name="Chart 15"/>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -17134,7 +17172,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="17" name="Chart 16"/>
+        <xdr:cNvPr id="17" name="Chart 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -17166,7 +17210,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="18" name="Chart 17"/>
+        <xdr:cNvPr id="18" name="Chart 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -17198,7 +17248,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="19" name="Chart 18"/>
+        <xdr:cNvPr id="19" name="Chart 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -17219,27 +17275,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_wDistinction_Full" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_wDistinction_Full" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Accuracy_wDistinction_PartialAsgmts" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_wDistinction_PartialClicks" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Fail_Sensitivity_wDistinction_PartialClicks" connectionId="48" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_wDistinction_PartialClicks" connectionId="42" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_wDistinction_Full" connectionId="40" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_wDistinction_Full" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_wDistinction_PartialClicks" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_wDistinction_PartialAsgmts" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Accuracy_wDistinction_PartialClicks" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17247,103 +17303,103 @@
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_wDistinction_Full" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_wDistinction_PartialAsgmts" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_wDistinction_PartialClicks" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_wDistinction_PartialClicks" connectionId="42" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_wDistinction_PartialAsgmts" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_wDistinction_PartialClicks" connectionId="36" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_wDistinction_PartialAsgmts" connectionId="41" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_wDistinction_Full" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_wDistinction_PartialAsgmts" connectionId="35" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Fail_Sensitivity_wDistinction_Full" connectionId="46" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Accuracy_wDistinction_PartialClicks" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_wDistinction_Full" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_wDistinction_PartialAsgmts" connectionId="41" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_wDistinction_PartialAsgmts" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Accuracy_wDistinction_Full" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_wDistinction_PartialClicks" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_wDistinction_PartialAsgmts" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_wDistinction_Full" connectionId="40" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_PartialAsgmts" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Fail_Sensitivity_Full" connectionId="43" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_PartialClicks" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_Full" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_PartialClicks" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_PartialClicks" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_PartialAsgmts" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_wDistinction_Full" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Fail_Sensitivity_PartialAsgmts" connectionId="44" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_PartialAsgmts" connectionId="38" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_PartialClicks" connectionId="39" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_PartialClicks" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_Full" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_Full" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_PartialAsgmts" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_PartialAsgmts" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_wDistinction_PartialAsgmts" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_Full" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Fail_Sensitivity_Full" connectionId="43" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_PartialClicks" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_PartialAsgmts" connectionId="38" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_PartialAsgmts" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_PartialAsgmts" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_Full" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_PartialClicks" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_PartialClicks" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Fail_Sensitivity_PartialClicks" connectionId="45" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17351,63 +17407,63 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Accuracy_wDistinction_PartialAsgmts" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_wDistinction_Full" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_PartialAsgmts" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Accuracy_Full" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Accuracy_PartialClicks" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_PartialAsgmts" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_Full" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable45.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_PartialClicks" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable46.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_PartialClicks" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable47.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_Full" connectionId="37" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Fail_Sensitivity_PartialAsgmts" connectionId="44" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Fail_Sensitivity_PartialClicks" connectionId="45" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_PartialClicks" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable45.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_Full" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable46.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Accuracy_PartialClicks" connectionId="39" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable47.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_Full" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable48.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Accuracy_Full" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_Full" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_wDistinction_PartialClicks" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Fail_Sensitivity_wDistinction_PartialAsgmts" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Fail_Sensitivity_wDistinction_PartialClicks" connectionId="36" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_Fail_Sensitivity_wDistinction_Full" connectionId="46" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LogReg_Accuracy_wDistinction_Full" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_wDistinction_PartialClicks" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Fail_Sensitivity_wDistinction_Full" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RF_Accuracy_wDistinction_Full" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_wDistinction_PartialClicks" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Bayes_Accuracy_wDistinction_PartialAsgmts" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17486,6 +17542,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -17521,6 +17594,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -17675,8 +17765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL83"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="U86" sqref="U86"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="AA74" sqref="AA74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22124,8 +22214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="Y74" sqref="Y74"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="U75" sqref="U75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>